<commit_message>
piece everything together with taking picture and plate detection
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -489,7 +489,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Wed Feb  8 18:26:19 2023</t>
+          <t>Thu Feb  9 08:50:17 2023</t>
         </is>
       </c>
     </row>
@@ -508,12 +508,68 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ABCD</t>
+          <t>29P188276</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Fri Feb 10 15:02:42 2023</t>
+          <t>Thu Feb  9 09:13:19 2023</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Thu Feb  9 09:13:19 2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>29P188276</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Thu Feb  9 09:13:43 2023</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Thu Feb  9 09:13:43 2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>123456789</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Fri Feb 10 09:56:40 2023</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Fri Feb 10 09:56:40 2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>123456789</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Fri Feb 10 10:04:28 2023</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Fri Feb 10 10:04:28 2023</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Final Push with everything together
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -573,6 +573,881 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>983106857623</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 00:42:30 2023</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 00:42:50 2023</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>test_plate.jpeg</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>test_plate.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>983106857623</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 01:47:30 2023</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 01:50:45 2023</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>test_plate1.jpeg</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>test_plate1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>899900581424</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 01:57:48 2023</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 01:57:53 2023</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>test_plate1.jpeg</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>test_plate1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>983106857623</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 01:57:54 2023</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 03:45:46 2023</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>test_plate1.jpeg</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>exit_test.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>899900581424</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 03:28:09 2023</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 03:29:18 2023</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>899900581424</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 03:29:48 2023</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 03:37:05 2023</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>exit_test.jpg</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>exit_test.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>899900581424</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 03:39:31 2023</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 10:59:57 2023</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>exit_test.jpg</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>exit_test.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>899900581424</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 11:00:47 2023</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 11:01:01 2023</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>exit_test.jpg</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>exit_test.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>899900581424</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 11:02:33 2023</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 11:02:47 2023</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>exit_test.jpg</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>exit_test.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>899900581424</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 11:02:56 2023</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 11:03:03 2023</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>exit_test.jpg</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>exit_test.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>899900581424</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 11:04:40 2023</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 11:04:46 2023</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>exit_test.jpg</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>exit_test.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>899900581424</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 11:05:22 2023</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 11:05:26 2023</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>exit_test.jpg</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>exit_test.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>899900581424</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 11:10:15 2023</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 11:12:25 2023</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>exit_test.jpg</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>exit_test.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>899900581424</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 11:12:33 2023</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 11:15:41 2023</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>exit_test.jpg</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>exit_test.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>899900581424</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 11:16:45 2023</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 11:19:42 2023</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>899900581424</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 11:19:49 2023</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 11:20:53 2023</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>899900581424</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 11:21:21 2023</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 11:22:51 2023</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>899900581424</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 11:22:58 2023</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 11:23:28 2023</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>899900581424</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 11:23:39 2023</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 13:18:31 2023</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>899900581424</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 13:19:14 2023</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 13:20:34 2023</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>899900581424</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 13:20:43 2023</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 13:24:36 2023</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>899900581424</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 13:24:40 2023</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 13:31:55 2023</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>899900581424</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 13:33:11 2023</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 13:35:55 2023</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>899900581424</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 13:36:01 2023</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 13:36:37 2023</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>899900581424</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 13:39:36 2023</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 13:41:04 2023</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>899900581424</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 13:41:36 2023</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 13:42:13 2023</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>899900581424</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 13:42:27 2023</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 13:45:56 2023</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>899900581424</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 13:46:05 2023</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 13:46:09 2023</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>899900581424</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 13:50:02 2023</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 13:50:22 2023</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>899900581424</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 13:50:28 2023</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 14:09:22 2023</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>899900581424</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 14:21:36 2023</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 14:21:45 2023</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>899900581424</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 14:22:25 2023</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 14:22:31 2023</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>899900581424</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 14:22:40 2023</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 14:22:56 2023</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>983106857623</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 14:22:44 2023</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 14:22:50 2023</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>899900581424</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 14:26:30 2023</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Sun Feb 12 14:26:35 2023</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>entry_test.jpg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>